<commit_message>
Updated the variance Logic and added test scnearios in test report.
</commit_message>
<xml_diff>
--- a/Test Data/ProdData.xlsx
+++ b/Test Data/ProdData.xlsx
@@ -19,27 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">This is the Prod Data for Demo Purpose </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 1 Containg 5 Columns and 3 rows </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>A1</t>
   </si>
   <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
     <t>A3</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>Table 3 Demo</t>
-  </si>
-  <si>
-    <t>Table 2 Demo</t>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
   </si>
   <si>
     <t>C1</t>
@@ -48,13 +51,10 @@
     <t>C2</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>Table 4 Demo</t>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
   <si>
     <t>D2</t>
@@ -64,15 +64,6 @@
   </si>
   <si>
     <t>D4</t>
-  </si>
-  <si>
-    <t>Table 5 Demo</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -117,16 +108,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -137,11 +128,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -362,199 +355,191 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3">
+        <v>25</v>
+      </c>
+      <c r="H6" s="4">
+        <v>113</v>
+      </c>
+      <c r="I6" s="4">
+        <v>228</v>
+      </c>
+      <c r="J6" s="4">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="3">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="3">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3">
+        <v>78</v>
+      </c>
+      <c r="F11" s="3">
+        <v>88</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="I12" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3">
+      <c r="J12" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="K12" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
+    <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="3">
         <v>10</v>
       </c>
-      <c r="G11" s="3">
-        <v>32</v>
-      </c>
-      <c r="H11" s="3">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="3">
-        <v>786</v>
-      </c>
-      <c r="D12" s="4">
-        <v>223</v>
-      </c>
-      <c r="G12" s="3">
-        <v>234</v>
-      </c>
-      <c r="H12" s="3">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="3">
-        <v>9088</v>
-      </c>
-      <c r="D13" s="4">
-        <v>3246</v>
-      </c>
-      <c r="G13" s="3">
-        <v>4234</v>
-      </c>
-      <c r="H13" s="3">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G14" s="3">
-        <v>3453</v>
-      </c>
+      <c r="I13" s="3">
+        <v>1200</v>
+      </c>
+      <c r="J13" s="3">
+        <v>14</v>
+      </c>
+      <c r="K13" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H14" s="3">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G15" s="3">
-        <v>324</v>
-      </c>
-      <c r="H15" s="3">
-        <v>5453</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="3">
-        <v>432</v>
-      </c>
-      <c r="C18" s="3">
-        <v>312</v>
-      </c>
-      <c r="D18" s="3">
-        <v>34554</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G19" s="3">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G20" s="3">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G21" s="3">
-        <v>3123</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G22" s="3">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G23" s="3">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="I14" s="3">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3">
+        <v>22</v>
+      </c>
+      <c r="K14" s="3">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Variance Code tested and stable
</commit_message>
<xml_diff>
--- a/Test Data/ProdData.xlsx
+++ b/Test Data/ProdData.xlsx
@@ -19,15 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
   <si>
     <t>A1</t>
   </si>
   <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A3</t>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
   <si>
     <t>B1</t>
@@ -39,31 +45,35 @@
     <t>C1</t>
   </si>
   <si>
+    <t>C2</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
     <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -112,11 +122,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,152 +352,212 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:H14"/>
+  <dimension ref="B3:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="F4" s="2">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
+    </row>
+    <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2">
+        <v>15</v>
+      </c>
+      <c r="I5" s="4">
+        <v>13</v>
+      </c>
+      <c r="J5" s="4">
+        <v>26</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>210</v>
+      </c>
+      <c r="C6" s="2">
+        <v>220</v>
+      </c>
+      <c r="D6" s="2">
+        <v>230</v>
+      </c>
+      <c r="E6" s="2">
+        <v>240</v>
+      </c>
+      <c r="F6" s="2">
+        <v>250</v>
+      </c>
+      <c r="I6" s="4">
+        <v>42</v>
+      </c>
+      <c r="J6" s="4">
+        <v>55</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
+      <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
+    </row>
+    <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="2">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2">
+        <v>37</v>
+      </c>
+      <c r="H11" s="2">
+        <v>119</v>
+      </c>
+      <c r="I11" s="2">
+        <v>122</v>
+      </c>
+      <c r="J11" s="2">
+        <v>133</v>
+      </c>
+      <c r="K11" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="2">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45</v>
+      </c>
+      <c r="E12" s="2">
+        <v>53</v>
+      </c>
+      <c r="H12" s="2">
+        <v>212</v>
+      </c>
+      <c r="I12" s="2">
+        <v>213</v>
+      </c>
+      <c r="J12" s="2">
+        <v>220</v>
+      </c>
+      <c r="K12" s="2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="2">
+        <v>3330</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3340</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3350</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
-        <v>200</v>
-      </c>
-      <c r="C6" s="3">
-        <v>200</v>
-      </c>
-      <c r="D6" s="3">
-        <v>200</v>
-      </c>
-      <c r="E6" s="3">
-        <v>200</v>
-      </c>
-      <c r="G6" s="4">
-        <v>113</v>
-      </c>
-      <c r="H6" s="4">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G7" s="3">
-        <v>200</v>
-      </c>
-      <c r="H7" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="3">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="3">
-        <v>200</v>
-      </c>
-      <c r="D11" s="3">
-        <v>200</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G12" s="3">
-        <v>12</v>
-      </c>
-      <c r="H12" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G13" s="3">
-        <v>10</v>
-      </c>
-      <c r="H13" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G14" s="3">
-        <v>200</v>
-      </c>
-      <c r="H14" s="3">
-        <v>200</v>
+    </row>
+    <row r="17" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="2">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="2">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="2">
+        <v>1237</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>